<commit_message>
Store hard-coded data in a .csv file.
</commit_message>
<xml_diff>
--- a/clientele.xlsx
+++ b/clientele.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plume\OneDrive\Dators\Hustle\Developing\python_solo_projects\clientele_accounting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675AEBBA-ED16-4D1A-9306-EDB9019C54F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2209C010-D122-4CA6-B330-A18112394413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9936" yWindow="1488" windowWidth="12216" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
     <t>service_type</t>
   </si>
   <si>
-    <t>notes</t>
+    <t>note</t>
   </si>
 </sst>
 </file>
@@ -380,7 +380,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>